<commit_message>
Att na planilha de requisitos das sprints
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Planilha de Requisitos Atualizada - SixSolutions (Sprint 2).xlsx
+++ b/Documentação/Planilhas/Planilha de Requisitos Atualizada - SixSolutions (Sprint 2).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Faculdade Breno\sixsolution\Sixsolution-project\Documentação\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B32141-7AFC-4275-8D67-B06F04DD0667}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5D8141-75C7-4795-8593-E310E3F97B80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{17B792A4-C0E8-4189-901C-A44B5E8E2A1C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Data da Sprint</t>
   </si>
@@ -166,6 +166,30 @@
   <si>
     <t>Será feito, estudado e 
 realizado por todos.</t>
+  </si>
+  <si>
+    <t>Site Institucional na Nuvem
+Cadastro, Login e Dashboard na Nuvem,                               conectado com BD                                                                                                     Mapeamento das tabelas (entidades) em classes Javascript</t>
+  </si>
+  <si>
+    <t>Fluxograma do Processo de Atendimento do Suporte
+Ferramenta de Help Desk configurada e integrada à solução</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                          Modelagem Lógica (Final)
+Script de criação do Banco (Final)
+Tabelas criadas no Azure (Final)
+</t>
+  </si>
+  <si>
+    <t>Teste Integrado do Analytics
+Teste Integrado da Solução de IoT                                         (Simulador + Banco de Dados)</t>
+  </si>
+  <si>
+    <t>Manual de Instalação
+ Doc. Final do Projeto
+ PPT da Apresentação do Projeto
+ Prévia (Demonstração da Solução + Apresentação)</t>
   </si>
 </sst>
 </file>
@@ -279,34 +303,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -623,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BF9A55D-4EA2-4178-84B5-CC0AAF6B2715}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,59 +679,59 @@
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="9">
         <v>44308</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="9"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="12"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="9"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="12"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="10"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="13"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="9">
         <v>44308</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="7"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="7"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="13"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -719,7 +743,7 @@
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="9">
         <v>44308</v>
       </c>
     </row>
@@ -727,7 +751,7 @@
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="13"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -739,7 +763,7 @@
       <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="9">
         <v>44308</v>
       </c>
     </row>
@@ -747,13 +771,13 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="12"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="13"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -762,27 +786,202 @@
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <v>44308</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="9">
+        <v>44357</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="11"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="9">
+        <v>44357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="10"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="9">
+        <v>44357</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="11"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="9">
+        <v>44357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="9">
+        <v>44357</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="10"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="40">
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="D9:D10"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="A6:A8"/>
@@ -790,19 +989,8 @@
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A2:A5"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="D9:D10"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>